<commit_message>
See test meta updates
</commit_message>
<xml_diff>
--- a/Excel Sheets/test meta.xlsx
+++ b/Excel Sheets/test meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\GitHub\meta-analysis\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF269A8E-D61B-4E4B-89E7-7D38E5A14AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8915A4D3-D094-46ED-803D-F3B26E1BFCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{A847AA46-0C10-4C95-BB1D-292B4EE4D696}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Paper</t>
   </si>
@@ -95,18 +95,12 @@
     <t>Garcia, JT. 2003</t>
   </si>
   <si>
-    <t>Part and Qvarnstrom 1997</t>
-  </si>
-  <si>
     <t>Dijkstra et al. 2017</t>
   </si>
   <si>
     <t>Whiting, MJ. 1999</t>
   </si>
   <si>
-    <t>Driessens et al. 2015</t>
-  </si>
-  <si>
     <t>Boerner and Kruger 2009</t>
   </si>
   <si>
@@ -168,6 +162,51 @@
   </si>
   <si>
     <t>Miyai et al. 2011</t>
+  </si>
+  <si>
+    <t>black/grey</t>
+  </si>
+  <si>
+    <t>acts</t>
+  </si>
+  <si>
+    <t>harriers (Circus pygargus)</t>
+  </si>
+  <si>
+    <t>harriers (Circus cyaneous)</t>
+  </si>
+  <si>
+    <t>black/rufus</t>
+  </si>
+  <si>
+    <t>cichlid fish Astatotilapia burtoni</t>
+  </si>
+  <si>
+    <t>xanthophore/melanocortin</t>
+  </si>
+  <si>
+    <t>dorsal color y/b</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>nr/min</t>
+  </si>
+  <si>
+    <t>attack rates</t>
+  </si>
+  <si>
+    <t>foreleg color painted unpainted</t>
+  </si>
+  <si>
+    <t>number of acts</t>
+  </si>
+  <si>
+    <t>lizard (Platysaurus broadleyi</t>
   </si>
 </sst>
 </file>
@@ -519,24 +558,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F504376F-99DA-45A6-A5CB-86F54770C5A8}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="25.6796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.04296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.04296875" customWidth="1"/>
     <col min="6" max="6" width="8.76953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,8 +609,11 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -605,80 +647,212 @@
       <c r="K2">
         <v>2.65</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0.77</v>
+      </c>
+      <c r="H3">
+        <v>0.3</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>0.39</v>
+      </c>
+      <c r="K3">
+        <v>0.3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>0.98</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>0.49</v>
+      </c>
+      <c r="H5">
+        <v>0.24</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>0.42</v>
+      </c>
+      <c r="K5">
+        <v>0.23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>3.08</v>
+      </c>
+      <c r="H6">
+        <v>0.59</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>3.46</v>
+      </c>
+      <c r="K6">
+        <v>0.61</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.75">
@@ -688,42 +862,42 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.75">
@@ -733,7 +907,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.75">
@@ -743,12 +917,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
See test meta and color xlsx
</commit_message>
<xml_diff>
--- a/Excel Sheets/test meta.xlsx
+++ b/Excel Sheets/test meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\GitHub\meta-analysis\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8915A4D3-D094-46ED-803D-F3B26E1BFCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B664458-9255-419D-A23D-E03C7B8BC321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{A847AA46-0C10-4C95-BB1D-292B4EE4D696}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Paper</t>
   </si>
@@ -101,12 +101,6 @@
     <t>Whiting, MJ. 1999</t>
   </si>
   <si>
-    <t>Boerner and Kruger 2009</t>
-  </si>
-  <si>
-    <t>Cassidy et al. 2017</t>
-  </si>
-  <si>
     <t>Yewers et al. 2016</t>
   </si>
   <si>
@@ -207,6 +201,21 @@
   </si>
   <si>
     <t>lizard (Platysaurus broadleyi</t>
+  </si>
+  <si>
+    <t>orange/yellow</t>
+  </si>
+  <si>
+    <t>lizard (Ctenophorus decresii)</t>
+  </si>
+  <si>
+    <t>yellow/orange grey</t>
+  </si>
+  <si>
+    <t>throat color</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -558,11 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F504376F-99DA-45A6-A5CB-86F54770C5A8}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -610,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.75">
@@ -648,7 +657,7 @@
         <v>2.65</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.75">
@@ -656,16 +665,16 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>6</v>
@@ -686,7 +695,7 @@
         <v>0.3</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.75">
@@ -694,16 +703,16 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4">
         <v>12</v>
@@ -724,7 +733,7 @@
         <v>0.1</v>
       </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.75">
@@ -732,16 +741,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -762,7 +771,7 @@
         <v>0.23</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.75">
@@ -770,13 +779,16 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -797,13 +809,25 @@
         <v>0.61</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>22</v>
       </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
@@ -822,17 +846,17 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.75">
@@ -847,77 +871,67 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>